<commit_message>
Editar y Eliminar materia registrada
Se crearon las funciones y los archivos necesarios para dar funcionalidad a la edición y eliminación de una materia registrada
</commit_message>
<xml_diff>
--- a/sgtcis/storage/archivos/plantilla_docentes.xlsx
+++ b/sgtcis/storage/archivos/plantilla_docentes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
   <si>
     <t>password</t>
   </si>
@@ -183,13 +183,22 @@
     <t>jorgetocto</t>
   </si>
   <si>
-    <t>paralelo</t>
-  </si>
-  <si>
     <t>ciclo</t>
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>paralelo_a</t>
+  </si>
+  <si>
+    <t>paralelo_b</t>
+  </si>
+  <si>
+    <t>paralelo_c</t>
+  </si>
+  <si>
+    <t>paralelo_d</t>
   </si>
 </sst>
 </file>
@@ -519,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,12 +540,13 @@
     <col min="2" max="2" width="27.140625" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -559,13 +569,22 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" t="s">
         <v>54</v>
       </c>
-      <c r="I1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -588,13 +607,22 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -617,13 +645,22 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -646,13 +683,22 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -675,13 +721,22 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -704,13 +759,22 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -733,13 +797,22 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -762,13 +835,22 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -791,13 +873,22 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -820,13 +911,22 @@
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J10" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -849,13 +949,22 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -878,13 +987,22 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" t="s">
+        <v>55</v>
+      </c>
+      <c r="L12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -907,10 +1025,19 @@
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I13" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="J13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K13" t="s">
+        <v>55</v>
+      </c>
+      <c r="L13" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solicitar tutoría - estudiante
se agregaron más funciones a la vista solicitar tutoria (para que le muestre al estudiante solamente las materias del ciclo y paralelo del que curso). Se modificó la presentación de la notificacion al docente.
</commit_message>
<xml_diff>
--- a/sgtcis/storage/archivos/plantilla_docentes.xlsx
+++ b/sgtcis/storage/archivos/plantilla_docentes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4200" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
   <si>
     <t>password</t>
   </si>
@@ -189,16 +189,10 @@
     <t>NA</t>
   </si>
   <si>
-    <t>paralelo_a</t>
-  </si>
-  <si>
-    <t>paralelo_b</t>
-  </si>
-  <si>
-    <t>paralelo_c</t>
-  </si>
-  <si>
-    <t>paralelo_d</t>
+    <t>paralelo</t>
+  </si>
+  <si>
+    <t>A,B</t>
   </si>
 </sst>
 </file>
@@ -528,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +540,7 @@
     <col min="8" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -572,19 +566,10 @@
         <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -607,22 +592,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
         <v>55</v>
       </c>
-      <c r="J2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -645,22 +621,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
         <v>55</v>
       </c>
-      <c r="J3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -683,22 +650,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s">
         <v>55</v>
       </c>
-      <c r="J4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -721,22 +679,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
         <v>55</v>
       </c>
-      <c r="J5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -759,22 +708,13 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I6" t="s">
         <v>55</v>
       </c>
-      <c r="J6" t="s">
-        <v>55</v>
-      </c>
-      <c r="K6" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -797,22 +737,13 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
         <v>55</v>
       </c>
-      <c r="J7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -835,22 +766,13 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s">
         <v>55</v>
       </c>
-      <c r="J8" t="s">
-        <v>55</v>
-      </c>
-      <c r="K8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -873,22 +795,13 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I9" t="s">
         <v>55</v>
       </c>
-      <c r="J9" t="s">
-        <v>55</v>
-      </c>
-      <c r="K9" t="s">
-        <v>55</v>
-      </c>
-      <c r="L9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -911,22 +824,13 @@
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
         <v>55</v>
       </c>
-      <c r="J10" t="s">
-        <v>55</v>
-      </c>
-      <c r="K10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -949,22 +853,13 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
         <v>55</v>
       </c>
-      <c r="J11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -987,22 +882,13 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I12" t="s">
         <v>55</v>
       </c>
-      <c r="J12" t="s">
-        <v>55</v>
-      </c>
-      <c r="K12" t="s">
-        <v>55</v>
-      </c>
-      <c r="L12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1025,18 +911,9 @@
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J13" t="s">
-        <v>55</v>
-      </c>
-      <c r="K13" t="s">
-        <v>55</v>
-      </c>
-      <c r="L13" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Diseños generales de toda la página
Se elaboraron algunos cambios de diseño a toda la página
</commit_message>
<xml_diff>
--- a/sgtcis/storage/archivos/plantilla_docentes.xlsx
+++ b/sgtcis/storage/archivos/plantilla_docentes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="101">
   <si>
     <t>password</t>
   </si>
@@ -42,154 +42,286 @@
     <t>is_estudiante</t>
   </si>
   <si>
-    <t>Cumbicus</t>
-  </si>
-  <si>
-    <t>Oscar</t>
-  </si>
-  <si>
-    <t>Valeria</t>
-  </si>
-  <si>
-    <t>Herrera</t>
-  </si>
-  <si>
-    <t>Roberto</t>
-  </si>
-  <si>
-    <t>Jácome</t>
-  </si>
-  <si>
-    <t>robertjacome@unl.edu.ec</t>
-  </si>
-  <si>
-    <t>valeriaherrera@unl.edu.ec</t>
-  </si>
-  <si>
-    <t>robertojacome</t>
+    <t>ciclo</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>paralelo</t>
+  </si>
+  <si>
+    <t>Angel Freddy</t>
+  </si>
+  <si>
+    <t>Ganazhapa Malla</t>
+  </si>
+  <si>
+    <t>angelganazhapa</t>
+  </si>
+  <si>
+    <t>Narvaez Guillen</t>
+  </si>
+  <si>
+    <t>Cristian Ramiro</t>
+  </si>
+  <si>
+    <t>cristiannarvaez</t>
+  </si>
+  <si>
+    <t>Edison Leonardo</t>
+  </si>
+  <si>
+    <t>Coronel Romero</t>
+  </si>
+  <si>
+    <t>edisoncoronel</t>
+  </si>
+  <si>
+    <t>Francisco Javier</t>
+  </si>
+  <si>
+    <t>Alvarez Pineda</t>
+  </si>
+  <si>
+    <t>franciscoalvarez</t>
+  </si>
+  <si>
+    <t>Gastón René</t>
+  </si>
+  <si>
+    <t>Chamba Romero</t>
+  </si>
+  <si>
+    <t>gastónchamba</t>
+  </si>
+  <si>
+    <t>Hernan Leonardo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torres Carrion </t>
+  </si>
+  <si>
+    <t>hernantorres</t>
+  </si>
+  <si>
+    <t>Javier Francisco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinche Freire </t>
+  </si>
+  <si>
+    <t>javiersinche</t>
+  </si>
+  <si>
+    <t>Jorge Iván</t>
+  </si>
+  <si>
+    <t>Tocto</t>
+  </si>
+  <si>
+    <t>jorgetocto</t>
+  </si>
+  <si>
+    <t>Jose Oswaldo</t>
+  </si>
+  <si>
+    <t>Guaman Quinche</t>
+  </si>
+  <si>
+    <t>joseguaman</t>
+  </si>
+  <si>
+    <t>Kelvin Armando</t>
+  </si>
+  <si>
+    <t>Alulima Carrion</t>
+  </si>
+  <si>
+    <t>kelvinalulima</t>
+  </si>
+  <si>
+    <t>Luis Antonio</t>
+  </si>
+  <si>
+    <t>Chamba Eras</t>
+  </si>
+  <si>
+    <t>luischamba</t>
+  </si>
+  <si>
+    <t>Luis Roberto</t>
+  </si>
+  <si>
+    <t>Jacome Galarza</t>
+  </si>
+  <si>
+    <t>Ruilova Sanchez</t>
+  </si>
+  <si>
+    <t>Mario Enrique</t>
+  </si>
+  <si>
+    <t>Cueva Hurtado</t>
+  </si>
+  <si>
+    <t>Marlon Santiago</t>
+  </si>
+  <si>
+    <t>Viñan Ludeña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nora Esperanza </t>
+  </si>
+  <si>
+    <t>Parra Celi</t>
+  </si>
+  <si>
+    <t>Oscar Miguel</t>
+  </si>
+  <si>
+    <t>Cumbicus Pineda</t>
+  </si>
+  <si>
+    <t>Pablo Fernando</t>
+  </si>
+  <si>
+    <t>Ordoñez Ordoñez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edwin Rene </t>
+  </si>
+  <si>
+    <t>Roberth Gustavo</t>
+  </si>
+  <si>
+    <t>Figueroa Diaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeria del Rosario </t>
+  </si>
+  <si>
+    <t>Herrera Salazar</t>
+  </si>
+  <si>
+    <t>Wilman Patricio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chamba Zaragocin </t>
+  </si>
+  <si>
+    <t>Ximena Yadira</t>
+  </si>
+  <si>
+    <t>Naranjo Ruiz</t>
+  </si>
+  <si>
+    <t>luisjacome</t>
+  </si>
+  <si>
+    <t>mariaruilova</t>
+  </si>
+  <si>
+    <t>mariocueva</t>
+  </si>
+  <si>
+    <t>marlonviñan</t>
+  </si>
+  <si>
+    <t>noraparra</t>
+  </si>
+  <si>
+    <t>oscarcumbicus</t>
+  </si>
+  <si>
+    <t>pabloordoñez</t>
+  </si>
+  <si>
+    <t>edwinguaman</t>
+  </si>
+  <si>
+    <t>roberthfigueroa</t>
   </si>
   <si>
     <t>valeriaherrera</t>
   </si>
   <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t>Chamba</t>
-  </si>
-  <si>
-    <t>luischamba@unl.edu.ec</t>
-  </si>
-  <si>
-    <t>luischamba</t>
-  </si>
-  <si>
-    <t>Gastón</t>
-  </si>
-  <si>
-    <t>gastonchamba@unl.edu.ec</t>
-  </si>
-  <si>
-    <t>gastonchamba</t>
-  </si>
-  <si>
-    <t>Robert</t>
-  </si>
-  <si>
-    <t>Figueroa</t>
-  </si>
-  <si>
-    <t>robertfigueroa@unl.edu.ec</t>
-  </si>
-  <si>
-    <t>robertfigueroa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marlon </t>
-  </si>
-  <si>
-    <t>Viñán</t>
-  </si>
-  <si>
-    <t>marlonvinan@unl.edu.ec</t>
-  </si>
-  <si>
-    <t>marlonviñan</t>
-  </si>
-  <si>
-    <t>Mario</t>
-  </si>
-  <si>
-    <t>Cueva</t>
-  </si>
-  <si>
-    <t>mariocueva@unl.edu.ec</t>
-  </si>
-  <si>
-    <t>mariocueva</t>
-  </si>
-  <si>
-    <t>Hernán</t>
-  </si>
-  <si>
-    <t>Torres</t>
-  </si>
-  <si>
-    <t>hernantorres@unl.edu.ec</t>
-  </si>
-  <si>
-    <t>hernantorres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alex </t>
-  </si>
-  <si>
-    <t>Padilla</t>
-  </si>
-  <si>
-    <t>alexpadilla@unl.edu.ec</t>
-  </si>
-  <si>
-    <t>alexpadilla</t>
-  </si>
-  <si>
-    <t>oscarcumbicus@unl.edu.ec</t>
-  </si>
-  <si>
-    <t>oscarcumbicus</t>
-  </si>
-  <si>
-    <t>Edison</t>
-  </si>
-  <si>
-    <t>Coronel</t>
-  </si>
-  <si>
-    <t>edisoncoronel@unl.edu.ec</t>
-  </si>
-  <si>
-    <t>edisoncoronel</t>
-  </si>
-  <si>
-    <t>Tocto</t>
-  </si>
-  <si>
-    <t>Jorge</t>
-  </si>
-  <si>
-    <t>jorgetocto@unl.edu.ec</t>
-  </si>
-  <si>
-    <t>jorgetocto</t>
-  </si>
-  <si>
-    <t>ciclo</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>paralelo</t>
+    <t>wilmanchamba</t>
+  </si>
+  <si>
+    <t>ximenanaranjo</t>
+  </si>
+  <si>
+    <t>angel.f.ganazhapa@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>cristian.narvaez@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>edison.coronel@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>fjalvarez@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>gaston.chamba@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>hltorres@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>javier.sinche@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>jorge.tocto@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>jose.o.guaman@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>kelvin.alulima@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>lachamba@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>lrjacome@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>Maria del Cisne</t>
+  </si>
+  <si>
+    <t>maria.ruilova.s@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>mecueva@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>marlon.vinan@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>nora.parra@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>oscar.cumbicus@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>pablo.ordonez@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>edwin.guaman@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>roberth.figueroa@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>vherrera@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>wpchamba@unl.edu.ec</t>
+  </si>
+  <si>
+    <t>ximena.naranjo@unl.edu.ec</t>
   </si>
 </sst>
 </file>
@@ -518,17 +650,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
@@ -559,25 +691,25 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
       <c r="E2">
         <v>0</v>
       </c>
@@ -588,24 +720,24 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -617,25 +749,25 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="I3" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
       <c r="E4">
         <v>0</v>
       </c>
@@ -646,25 +778,25 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="I4" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
       <c r="E5">
         <v>0</v>
       </c>
@@ -675,25 +807,25 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
       <c r="E6">
         <v>0</v>
       </c>
@@ -704,24 +836,24 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -733,24 +865,24 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -762,24 +894,24 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -791,24 +923,24 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -820,24 +952,24 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="I10" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -849,24 +981,24 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -878,57 +1010,387 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="I12" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>52</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="C18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
         <v>55</v>
       </c>
-      <c r="I13" t="s">
-        <v>55</v>
+      <c r="C19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C2" r:id="rId1" display="mailto:angel.f.ganazhapa@unl.edu.ec"/>
+    <hyperlink ref="C3" r:id="rId2" display="mailto:cristian.narvaez@unl.edu.ec"/>
+    <hyperlink ref="C4" r:id="rId3" display="mailto:edison.coronel@unl.edu.ec"/>
+    <hyperlink ref="C5" r:id="rId4" display="mailto:fjalvarez@unl.edu.ec"/>
+    <hyperlink ref="C6" r:id="rId5" display="mailto:gaston.chamba@unl.edu.ec"/>
+    <hyperlink ref="C7" r:id="rId6" display="mailto:hltorres@unl.edu.ec"/>
+    <hyperlink ref="C8" r:id="rId7" display="mailto:javier.sinche@unl.edu.ec"/>
+    <hyperlink ref="C9" r:id="rId8" display="mailto:jorge.tocto@unl.edu.ec"/>
+    <hyperlink ref="C10" r:id="rId9" display="mailto:jose.o.guaman@unl.edu.ec"/>
+    <hyperlink ref="C11" r:id="rId10" display="mailto:kelvin.alulima@unl.edu.ec"/>
+    <hyperlink ref="C12" r:id="rId11" display="mailto:lachamba@unl.edu.ec"/>
+    <hyperlink ref="C13" r:id="rId12" display="mailto:lrjacome@unl.edu.ec"/>
+    <hyperlink ref="C14" r:id="rId13" display="mailto:maria.ruilova.s@unl.edu.ec"/>
+    <hyperlink ref="C15" r:id="rId14" display="mailto:mecueva@unl.edu.ec"/>
+    <hyperlink ref="C16" r:id="rId15" display="mailto:marlon.vinan@unl.edu.ec"/>
+    <hyperlink ref="C17" r:id="rId16" display="mailto:nora.parra@unl.edu.ec"/>
+    <hyperlink ref="C18" r:id="rId17" display="mailto:oscar.cumbicus@unl.edu.ec"/>
+    <hyperlink ref="C19" r:id="rId18" display="mailto:pablo.ordonez@unl.edu.ec"/>
+    <hyperlink ref="C20" r:id="rId19" display="mailto:edwin.guaman@unl.edu.ec"/>
+    <hyperlink ref="C21" r:id="rId20" display="mailto:roberth.figueroa@unl.edu.ec"/>
+    <hyperlink ref="C22" r:id="rId21" display="mailto:vherrera@unl.edu.ec"/>
+    <hyperlink ref="C23" r:id="rId22" display="mailto:wpchamba@unl.edu.ec"/>
+    <hyperlink ref="C24" r:id="rId23" display="mailto:ximena.naranjo@unl.edu.ec"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>